<commit_message>
- Nouvelle version des fichiers de la paroisse 3040.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20901 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 3/3040/group.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 3/3040/group.xlsx
@@ -2,26 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="7020" windowWidth="29745" windowHeight="13275" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="6735" windowWidth="1980" windowHeight="14175"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuille1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuille1!$A$1:$I$1</definedName>
+  </definedNames>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
-    <t>_id</t>
+    <t>_Id</t>
   </si>
   <si>
     <t>IdxPar</t>
@@ -36,7 +34,7 @@
     <t>IdxSG</t>
   </si>
   <si>
-    <t>ListSG::DesSG</t>
+    <t>DesSG</t>
   </si>
   <si>
     <t>c</t>
@@ -126,6 +124,9 @@
     <t>St-Etienne / Locataire</t>
   </si>
   <si>
+    <t>St-Etienne / Donateur</t>
+  </si>
+  <si>
     <t>Vente / Service</t>
   </si>
   <si>
@@ -133,9 +134,6 @@
   </si>
   <si>
     <t>Calendrier</t>
-  </si>
-  <si>
-    <t>St-Etienne / Donateur</t>
   </si>
   <si>
     <t>Croire</t>
@@ -169,37 +167,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color indexed="72"/>
+      <name val="Verdana"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color indexed="72"/>
+      <name val="Verdana"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,43 +199,94 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00DD0806"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -588,14 +619,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="7" width="21.85546875" style="2"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="20.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -621,878 +649,928 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>19271</v>
-      </c>
-      <c r="B2" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="A2" s="2">
+        <v>23084</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C2" s="2">
         <v>403110101</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="7">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2">
         <v>403110100</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>19272</v>
-      </c>
-      <c r="B3" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="A3" s="2">
+        <v>23085</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C3" s="2">
         <v>403110102</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="7">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2">
         <v>403110100</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>19273</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="A4" s="2">
+        <v>23086</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C4" s="2">
         <v>403110103</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2">
         <v>403110100</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>19274</v>
-      </c>
-      <c r="B5" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="A5" s="2">
+        <v>23087</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C5" s="2">
         <v>403110104</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2">
         <v>403110100</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>19275</v>
-      </c>
-      <c r="B6" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="A6" s="2">
+        <v>23088</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C6" s="2">
         <v>403110105</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="7">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2">
         <v>403110100</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>19276</v>
-      </c>
-      <c r="B7" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="A7" s="2">
+        <v>23089</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C7" s="2">
         <v>403110106</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="7">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2">
         <v>403110100</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>19277</v>
-      </c>
-      <c r="B8" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="A8" s="2">
+        <v>23090</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C8" s="2">
         <v>403110107</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2">
         <v>403110100</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>19278</v>
-      </c>
-      <c r="B9" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="A9" s="2">
+        <v>23091</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C9" s="2">
         <v>403110201</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2">
         <v>403110200</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>19279</v>
-      </c>
-      <c r="B10" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="A10" s="2">
+        <v>23092</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C10" s="2">
         <v>403110202</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2">
         <v>403110200</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>19280</v>
-      </c>
-      <c r="B11" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="A11" s="2">
+        <v>23093</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C11" s="2">
         <v>403110203</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2">
         <v>403110200</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>19281</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="A12" s="2">
+        <v>23094</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C12" s="2">
         <v>403110204</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2">
         <v>403110200</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>19282</v>
-      </c>
-      <c r="B13" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="A13" s="2">
+        <v>23095</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C13" s="2">
         <v>403110205</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="2">
         <v>403110200</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>19283</v>
-      </c>
-      <c r="B14" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="A14" s="2">
+        <v>23096</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C14" s="2">
         <v>403110206</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="2">
         <v>403110200</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>19284</v>
-      </c>
-      <c r="B15" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="A15" s="2">
+        <v>23097</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C15" s="2">
         <v>403110207</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="2">
         <v>403110200</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>19285</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="A16" s="2">
+        <v>23098</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C16" s="2">
         <v>403110208</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="2">
         <v>403110200</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>19286</v>
-      </c>
-      <c r="B17" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="A17" s="2">
+        <v>23099</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C17" s="2">
         <v>403110209</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="7">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2">
         <v>403110200</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>19287</v>
-      </c>
-      <c r="B18" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="A18" s="2">
+        <v>23100</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C18" s="2">
         <v>403110210</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="7">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2">
         <v>403110200</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>19288</v>
-      </c>
-      <c r="B19" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="A19" s="2">
+        <v>23101</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C19" s="2">
         <v>403110211</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="7">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="2">
         <v>403110200</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>19289</v>
-      </c>
-      <c r="B20" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="A20" s="2">
+        <v>23102</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C20" s="2">
         <v>403110212</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="2">
         <v>403110200</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>19290</v>
-      </c>
-      <c r="B21" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="A21" s="2">
+        <v>23103</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C21" s="2">
         <v>403110213</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="2">
         <v>403110200</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>19291</v>
-      </c>
-      <c r="B22" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="A22" s="2">
+        <v>23104</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C22" s="2">
         <v>403110214</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="7">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2">
         <v>403110200</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>19292</v>
-      </c>
-      <c r="B23" s="4">
-        <v>3040000000</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="A23" s="2">
+        <v>23105</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3040000000</v>
+      </c>
+      <c r="C23" s="2">
         <v>403110215</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="7">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="2">
         <v>403110200</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>19293</v>
-      </c>
-      <c r="B24" s="7">
+      <c r="A24" s="2">
+        <v>23106</v>
+      </c>
+      <c r="B24" s="2">
         <v>3040000000</v>
       </c>
       <c r="C24" s="2">
-        <v>403110216</v>
-      </c>
-      <c r="D24" s="2" t="s">
+        <v>403110316</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="2">
         <v>403110300</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>19294</v>
-      </c>
-      <c r="B25" s="7">
+      <c r="A25" s="2">
+        <v>23107</v>
+      </c>
+      <c r="B25" s="2">
         <v>3040000000</v>
       </c>
       <c r="C25" s="2">
-        <v>403110217</v>
-      </c>
-      <c r="D25" s="2" t="s">
+        <v>403110317</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="2">
         <v>403110300</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <v>19295</v>
-      </c>
-      <c r="B26" s="7">
+      <c r="A26" s="2">
+        <v>23108</v>
+      </c>
+      <c r="B26" s="2">
         <v>3040000000</v>
       </c>
       <c r="C26" s="2">
-        <v>403110218</v>
-      </c>
-      <c r="D26" s="2" t="s">
+        <v>403110318</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="2">
         <v>403110300</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <v>19296</v>
-      </c>
-      <c r="B27" s="7">
+      <c r="A27" s="2">
+        <v>23109</v>
+      </c>
+      <c r="B27" s="2">
         <v>3040000000</v>
       </c>
       <c r="C27" s="2">
-        <v>403110219</v>
-      </c>
-      <c r="D27" s="2" t="s">
+        <v>403110319</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="2">
         <v>403110300</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <v>19297</v>
-      </c>
-      <c r="B28" s="7">
+      <c r="A28" s="2">
+        <v>23110</v>
+      </c>
+      <c r="B28" s="2">
         <v>3040000000</v>
       </c>
       <c r="C28" s="2">
-        <v>403110220</v>
-      </c>
-      <c r="D28" s="2" t="s">
+        <v>403110320</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
       <c r="H28" s="2">
         <v>403110300</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
-        <v>19298</v>
-      </c>
-      <c r="B29" s="7">
+      <c r="A29" s="2">
+        <v>23111</v>
+      </c>
+      <c r="B29" s="2">
         <v>3040000000</v>
       </c>
       <c r="C29" s="2">
-        <v>403110221</v>
-      </c>
-      <c r="D29" s="2" t="s">
+        <v>403110321</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="2">
         <v>403110300</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
-        <v>19299</v>
-      </c>
-      <c r="B30" s="7">
+      <c r="A30" s="2">
+        <v>23112</v>
+      </c>
+      <c r="B30" s="2">
         <v>3040000000</v>
       </c>
       <c r="C30" s="2">
-        <v>403110223</v>
-      </c>
-      <c r="D30" s="2" t="s">
+        <v>403110322</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="2">
         <v>403110300</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>19300</v>
-      </c>
-      <c r="B31" s="7">
+      <c r="A31" s="2">
+        <v>23113</v>
+      </c>
+      <c r="B31" s="2">
         <v>3040000000</v>
       </c>
       <c r="C31" s="2">
-        <v>403110224</v>
-      </c>
-      <c r="D31" s="2" t="s">
+        <v>403110323</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="2">
         <v>403110300</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <v>19301</v>
-      </c>
-      <c r="B32" s="7">
+      <c r="A32" s="2">
+        <v>23114</v>
+      </c>
+      <c r="B32" s="2">
         <v>3040000000</v>
       </c>
       <c r="C32" s="2">
-        <v>403110227</v>
-      </c>
-      <c r="D32" s="2" t="s">
+        <v>403110324</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="2">
         <v>403110300</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <v>19302</v>
-      </c>
-      <c r="B33" s="7">
+      <c r="A33" s="2">
+        <v>23115</v>
+      </c>
+      <c r="B33" s="2">
         <v>3040000000</v>
       </c>
       <c r="C33" s="2">
-        <v>403110222</v>
-      </c>
-      <c r="D33" s="2" t="s">
+        <v>403110327</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="2">
         <v>403110300</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
-        <v>19303</v>
-      </c>
-      <c r="B34" s="7">
+      <c r="A34" s="2">
+        <v>23116</v>
+      </c>
+      <c r="B34" s="2">
         <v>3040000000</v>
       </c>
       <c r="C34" s="2">
-        <v>403110228</v>
-      </c>
-      <c r="D34" s="2" t="s">
+        <v>403110328</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="2">
         <v>403110300</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>19304</v>
-      </c>
-      <c r="B35" s="7">
+      <c r="A35" s="2">
+        <v>23117</v>
+      </c>
+      <c r="B35" s="2">
         <v>3040000000</v>
       </c>
       <c r="C35" s="2">
-        <v>403110235</v>
-      </c>
-      <c r="D35" s="2" t="s">
+        <v>403110335</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
       <c r="H35" s="2">
         <v>403110300</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <v>19305</v>
-      </c>
-      <c r="B36" s="7">
+      <c r="A36" s="2">
+        <v>23118</v>
+      </c>
+      <c r="B36" s="2">
         <v>3040000000</v>
       </c>
       <c r="C36" s="2">
-        <v>403110237</v>
-      </c>
-      <c r="D36" s="2" t="s">
+        <v>403110337</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
       <c r="H36" s="2">
         <v>403110300</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I36" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <v>19306</v>
-      </c>
-      <c r="B37" s="7">
+      <c r="A37" s="2">
+        <v>23119</v>
+      </c>
+      <c r="B37" s="2">
         <v>3040000000</v>
       </c>
       <c r="C37" s="2">
-        <v>403110238</v>
-      </c>
-      <c r="D37" s="2" t="s">
+        <v>403110338</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
       <c r="H37" s="2">
         <v>403110300</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I37" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <v>19307</v>
-      </c>
-      <c r="B38" s="7">
+      <c r="A38" s="2">
+        <v>23120</v>
+      </c>
+      <c r="B38" s="2">
         <v>3040000000</v>
       </c>
       <c r="C38" s="2">
-        <v>403110239</v>
-      </c>
-      <c r="D38" s="2" t="s">
+        <v>403110439</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
       <c r="H38" s="2">
         <v>403110400</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
-        <v>19308</v>
-      </c>
-      <c r="B39" s="7">
+      <c r="A39" s="2">
+        <v>23121</v>
+      </c>
+      <c r="B39" s="2">
         <v>3040000000</v>
       </c>
       <c r="C39" s="2">
-        <v>403110240</v>
-      </c>
-      <c r="D39" s="2" t="s">
+        <v>403110540</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
       <c r="H39" s="2">
         <v>403110500</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
-        <v>19309</v>
-      </c>
-      <c r="B40" s="7">
+      <c r="A40" s="2">
+        <v>23122</v>
+      </c>
+      <c r="B40" s="2">
         <v>3040000000</v>
       </c>
       <c r="C40" s="2">
-        <v>403110243</v>
-      </c>
-      <c r="D40" s="2" t="s">
+        <v>403110343</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
       <c r="H40" s="2">
         <v>403110300</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
-        <v>19310</v>
-      </c>
-      <c r="B41" s="7">
+      <c r="A41" s="2">
+        <v>23123</v>
+      </c>
+      <c r="B41" s="2">
         <v>3040000000</v>
       </c>
       <c r="C41" s="2">
-        <v>403110244</v>
-      </c>
-      <c r="D41" s="2" t="s">
+        <v>403110344</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="2">
         <v>403110300</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="3" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>